<commit_message>
updated: excel Draft Perhitungan dengan Jaminan Pensiun
</commit_message>
<xml_diff>
--- a/case_study_IRR_rate/Draft Perhitungan.xlsx
+++ b/case_study_IRR_rate/Draft Perhitungan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZakiZ\Downloads\teori dana pensiun\teori-dana-pensiun\case_study_IRR_rate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB04903C-3F5C-41A7-8A9F-8475F12834D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E59EA9-6278-4CA6-B57D-9D4FF8BFE8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{7B0AFCA6-860D-478D-9BA3-BF4DD6D924DF}"/>
   </bookViews>
@@ -19,15 +19,21 @@
     <sheet name="Hasil &amp; Solusi" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="Batas_Atas_Manfaat_JP">Asumsi!$B$15</definedName>
+    <definedName name="Faktor_Anuitas_60">'Tabel Mortalita'!$E$2</definedName>
     <definedName name="Gaji_Awal">Asumsi!$B$4</definedName>
     <definedName name="Gender">Asumsi!$B$5</definedName>
     <definedName name="Imbal_Hasil">Asumsi!$B$7</definedName>
     <definedName name="Kenaikan_Gaji">Asumsi!$B$6</definedName>
+    <definedName name="Manfaat_JP_Final">'Hasil &amp; Solusi'!$B$16</definedName>
+    <definedName name="Masa_Iuran_JP">'Hasil &amp; Solusi'!$B$15</definedName>
     <definedName name="Masa_Kerja">Asumsi!$B$11</definedName>
     <definedName name="Rate_Iuran_JHT">Asumsi!$B$9</definedName>
     <definedName name="Target_IRR">Asumsi!$B$8</definedName>
     <definedName name="Usia_Awal">Asumsi!$B$2</definedName>
+    <definedName name="Usia_Mulai_Iuran_JP">Asumsi!$B$14</definedName>
     <definedName name="Usia_Pensiun">Asumsi!$B$3</definedName>
+    <definedName name="Usia_Pensiun_JP">Asumsi!$B$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Variabel Input</t>
   </si>
@@ -172,14 +178,45 @@
   <si>
     <t>IURAN DPLK BULANAN YANG DIPERLUKAN</t>
   </si>
+  <si>
+    <t>Usia Pensiun JP (Tahun)</t>
+  </si>
+  <si>
+    <t>Usia Mulai Iuran JP (Tahun)</t>
+  </si>
+  <si>
+    <t>Batas Atas Manfaat JP (Bulanan)</t>
+  </si>
+  <si>
+    <t>Jumlah Seluruh PV Anuitas</t>
+  </si>
+  <si>
+    <t>Faktor Anuitas Hidup (ä_60)</t>
+  </si>
+  <si>
+    <t>Perhitungan Manfaat Jaminan Pensiun (JP)</t>
+  </si>
+  <si>
+    <t>Masa Iuran JP (Bulan)</t>
+  </si>
+  <si>
+    <t>Manfaat JP Final (Bulanan)</t>
+  </si>
+  <si>
+    <t>Nilai Lump Sum JP di Usia 60</t>
+  </si>
+  <si>
+    <t>PV Manfaat JP di Usia 55</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$Rp-421]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$Rp-421]#,##0"/>
+    <numFmt numFmtId="173" formatCode="_-[$Rp-3809]* #,##0.00_-;\-[$Rp-3809]* #,##0.00_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -198,12 +235,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -218,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -237,6 +280,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,16 +616,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612C0063-8236-46AF-AC5F-96BDF0ECC8EA}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -666,6 +711,30 @@
       <c r="B11" s="2">
         <f>B3-B2</f>
         <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="10">
+        <v>4792300</v>
       </c>
     </row>
   </sheetData>
@@ -1442,15 +1511,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313B0484-5A8B-48F7-A5D2-4BF4108AA8A9}">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
@@ -1462,6 +1531,9 @@
       <c r="B1" t="s">
         <v>19</v>
       </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
       <c r="E1">
         <f>SUM(F57:F113)</f>
         <v>13.375236131676656</v>
@@ -1474,6 +1546,13 @@
       <c r="B2">
         <v>100000</v>
       </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2">
+        <f>SUM(J62:J113)</f>
+        <v>12.566322375149717</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1843,7 +1922,7 @@
         <v>95980.11264543749</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1851,7 +1930,7 @@
         <v>95655.699864695911</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1859,7 +1938,7 @@
         <v>95295.077876206007</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1867,7 +1946,7 @@
         <v>94896.744450683473</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1875,7 +1954,7 @@
         <v>94459.270458765823</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1883,7 +1962,7 @@
         <v>93979.417364835288</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1891,7 +1970,7 @@
         <v>93456.891804286803</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1899,7 +1978,7 @@
         <v>92887.739333198697</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1919,7 +1998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1942,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1966,7 +2045,7 @@
         <v>0.93595283018867914</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1990,7 +2069,7 @@
         <v>0.87549557520469901</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2014,7 +2093,7 @@
         <v>0.8185222876786421</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2038,7 +2117,7 @@
         <v>0.7649399654691883</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2061,8 +2140,23 @@
         <f t="shared" si="3"/>
         <v>0.71463433811743637</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <f>B62/$B$62</f>
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <f>(1/(1+Imbal_Hasil))^G62</f>
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <f>I62*H62</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2085,8 +2179,24 @@
         <f t="shared" si="3"/>
         <v>0.66744824630154986</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <f>G62+1</f>
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <f>B63/$B$62</f>
+        <v>0.99000999999999995</v>
+      </c>
+      <c r="I63">
+        <f>(1/(1+Imbal_Hasil))^G63</f>
+        <v>0.94339622641509424</v>
+      </c>
+      <c r="J63">
+        <f>I63*H63</f>
+        <v>0.93397169811320735</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2109,8 +2219,24 @@
         <f t="shared" si="3"/>
         <v>0.62322035496171879</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <f t="shared" ref="G64:G113" si="4">G63+1</f>
+        <v>2</v>
+      </c>
+      <c r="H64">
+        <f t="shared" ref="H64:H113" si="5">B64/$B$62</f>
+        <v>0.97987229759999983</v>
+      </c>
+      <c r="I64">
+        <f>(1/(1+Imbal_Hasil))^G64</f>
+        <v>0.88999644001423972</v>
+      </c>
+      <c r="J64">
+        <f t="shared" ref="J64:J113" si="6">I64*H64</f>
+        <v>0.87208285653257345</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2133,8 +2259,24 @@
         <f t="shared" si="3"/>
         <v>0.58179383966869724</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="5"/>
+        <v>0.96962283336710375</v>
+      </c>
+      <c r="I65">
+        <f>(1/(1+Imbal_Hasil))^G65</f>
+        <v>0.83961928303230149</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="6"/>
+        <v>0.81411402816343637</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2157,8 +2299,24 @@
         <f t="shared" si="3"/>
         <v>0.54298379966589194</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="5"/>
+        <v>0.95923817282174217</v>
+      </c>
+      <c r="I66">
+        <f>(1/(1+Imbal_Hasil))^G66</f>
+        <v>0.79209366323802022</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="6"/>
+        <v>0.75980647822811886</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2181,8 +2339,24 @@
         <f t="shared" si="3"/>
         <v>0.506593640110925</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="5"/>
+        <v>0.94864818339379009</v>
+      </c>
+      <c r="I67">
+        <f>(1/(1+Imbal_Hasil))^G67</f>
+        <v>0.74725817286605678</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="6"/>
+        <v>0.70888510821554751</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2205,8 +2379,24 @@
         <f t="shared" si="3"/>
         <v>0.47244158207099402</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="5"/>
+        <v>0.93777667521209718</v>
+      </c>
+      <c r="I68">
+        <f>(1/(1+Imbal_Hasil))^G68</f>
+        <v>0.70496054043967604</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="6"/>
+        <v>0.66109555176924262</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2229,8 +2419,24 @@
         <f t="shared" si="3"/>
         <v>0.4403556674546818</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="5"/>
+        <v>0.92653273287630422</v>
+      </c>
+      <c r="I69">
+        <f>(1/(1+Imbal_Hasil))^G69</f>
+        <v>0.66505711362233577</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="6"/>
+        <v>0.61619718500332954</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2253,8 +2459,24 @@
         <f t="shared" si="3"/>
         <v>0.41019545853278566</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="5"/>
+        <v>0.91485842044206278</v>
+      </c>
+      <c r="I70">
+        <f>(1/(1+Imbal_Hasil))^G70</f>
+        <v>0.62741237134182615</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="6"/>
+        <v>0.57399349101159203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -2277,8 +2499,24 @@
         <f t="shared" si="3"/>
         <v>0.3818339253668725</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="5"/>
+        <v>0.90269995203438769</v>
+      </c>
+      <c r="I71">
+        <f>(1/(1+Imbal_Hasil))^G71</f>
+        <v>0.59189846353002462</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="6"/>
+        <v>0.53430671463778101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -2301,8 +2539,24 @@
         <f t="shared" si="3"/>
         <v>0.35515958369383754</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="5"/>
+        <v>0.89001701770830455</v>
+      </c>
+      <c r="I72">
+        <f>(1/(1+Imbal_Hasil))^G72</f>
+        <v>0.55839477691511752</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="6"/>
+        <v>0.49698085405388692</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2325,8 +2579,24 @@
         <f t="shared" si="3"/>
         <v>0.33008062629809815</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="5"/>
+        <v>0.87680026499533614</v>
+      </c>
+      <c r="I73">
+        <f>(1/(1+Imbal_Hasil))^G73</f>
+        <v>0.52678752539162021</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="6"/>
+        <v>0.46188744185960995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2349,8 +2619,24 @@
         <f t="shared" si="3"/>
         <v>0.30649543135864721</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="5"/>
+        <v>0.86299942882430958</v>
+      </c>
+      <c r="I74">
+        <f>(1/(1+Imbal_Hasil))^G74</f>
+        <v>0.49696936357700011</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="6"/>
+        <v>0.42888427691013176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -2373,8 +2659,24 @@
         <f t="shared" si="3"/>
         <v>0.28431788458014878</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="5"/>
+        <v>0.84858733836294353</v>
+      </c>
+      <c r="I75">
+        <f>(1/(1+Imbal_Hasil))^G75</f>
+        <v>0.46883902224245294</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="6"/>
+        <v>0.39785085800540804</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -2397,8 +2699,24 @@
         <f t="shared" si="3"/>
         <v>0.263458071482226</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="5"/>
+        <v>0.83350794136023409</v>
+      </c>
+      <c r="I76">
+        <f>(1/(1+Imbal_Hasil))^G76</f>
+        <v>0.44230096437967248</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="6"/>
+        <v>0.36866136628174706</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2421,8 +2739,24 @@
         <f t="shared" si="3"/>
         <v>0.24383541606380921</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G77">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="5"/>
+        <v>0.81771296587145759</v>
+      </c>
+      <c r="I77">
+        <f>(1/(1+Imbal_Hasil))^G77</f>
+        <v>0.41726506073553998</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="6"/>
+        <v>0.34120305036859228</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2445,8 +2779,24 @@
         <f t="shared" si="3"/>
         <v>0.22537293446637399</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="5"/>
+        <v>0.80114610118290186</v>
+      </c>
+      <c r="I78">
+        <f>(1/(1+Imbal_Hasil))^G78</f>
+        <v>0.39364628371277355</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="6"/>
+        <v>0.31536818544162698</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -2469,8 +2819,24 @@
         <f t="shared" si="3"/>
         <v>0.20757910344232597</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G79">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="5"/>
+        <v>0.78216695004587888</v>
+      </c>
+      <c r="I79">
+        <f>(1/(1+Imbal_Hasil))^G79</f>
+        <v>0.37136441859695613</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="6"/>
+        <v>0.29046897464954224</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -2493,8 +2859,24 @@
         <f t="shared" si="3"/>
         <v>0.19046753546233497</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="5"/>
+        <v>0.76075121895362274</v>
+      </c>
+      <c r="I80">
+        <f>(1/(1+Imbal_Hasil))^G80</f>
+        <v>0.35034379112920383</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="6"/>
+        <v>0.26652446615437519</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -2517,8 +2899,24 @@
         <f t="shared" si="3"/>
         <v>0.17406217132298479</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="5"/>
+        <v>0.73693970580037438</v>
+      </c>
+      <c r="I81">
+        <f>(1/(1+Imbal_Hasil))^G81</f>
+        <v>0.33051301049924886</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="6"/>
+        <v>0.24356816072051252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -2541,8 +2939,24 @@
         <f t="shared" si="3"/>
         <v>0.15814533522266697</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="5"/>
+        <v>0.7097245224651666</v>
+      </c>
+      <c r="I82">
+        <f>(1/(1+Imbal_Hasil))^G82</f>
+        <v>0.31180472688608379</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="6"/>
+        <v>0.22129546089160751</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2565,8 +2979,24 @@
         <f t="shared" si="3"/>
         <v>0.1424531405446291</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G83">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="5"/>
+        <v>0.67765916854019037</v>
+      </c>
+      <c r="I83">
+        <f>(1/(1+Imbal_Hasil))^G83</f>
+        <v>0.29415540272272056</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="6"/>
+        <v>0.19933710563068366</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2589,8 +3019,24 @@
         <f t="shared" si="3"/>
         <v>0.12696203345917681</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="5"/>
+        <v>0.64020494629497404</v>
+      </c>
+      <c r="I84">
+        <f>(1/(1+Imbal_Hasil))^G84</f>
+        <v>0.27750509690822689</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="6"/>
+        <v>0.17766013566271296</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2613,8 +3059,24 @@
         <f t="shared" si="3"/>
         <v>0.11171221638368395</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="5"/>
+        <v>0.5971063493103963</v>
+      </c>
+      <c r="I85">
+        <f>(1/(1+Imbal_Hasil))^G85</f>
+        <v>0.26179726123417624</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="6"/>
+        <v>0.15632080691499911</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2637,8 +3099,24 @@
         <f t="shared" si="3"/>
         <v>9.6717486056258892E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="5"/>
+        <v>0.54797643888913694</v>
+      </c>
+      <c r="I86">
+        <f>(1/(1+Imbal_Hasil))^G86</f>
+        <v>0.24697854833412852</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="6"/>
+        <v>0.13533842539814434</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2661,8 +3139,24 @@
         <f t="shared" si="3"/>
         <v>8.2594908233817613E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="5"/>
+        <v>0.49603923201122452</v>
+      </c>
+      <c r="I87">
+        <f>(1/(1+Imbal_Hasil))^G87</f>
+        <v>0.23299863050389483</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="6"/>
+        <v>0.11557646173481906</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2685,8 +3179,24 @@
         <f t="shared" si="3"/>
         <v>6.9765425553913768E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="5"/>
+        <v>0.44412872638124989</v>
+      </c>
+      <c r="I88">
+        <f>(1/(1+Imbal_Hasil))^G88</f>
+        <v>0.21981002877725925</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="6"/>
+        <v>9.7623948126670038E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2702,15 +3212,31 @@
         <v>0.37575379114410867</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89:E113" si="4">(1/(1+Imbal_Hasil))^C89</f>
+        <f t="shared" ref="E89:E113" si="7">(1/(1+Imbal_Hasil))^C89</f>
         <v>0.15495739668087741</v>
       </c>
       <c r="F89">
         <f t="shared" si="3"/>
         <v>5.8225829268661211E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G89">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="5"/>
+        <v>0.3929073603677003</v>
+      </c>
+      <c r="I89">
+        <f>(1/(1+Imbal_Hasil))^G89</f>
+        <v>0.20736795167665964</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="6"/>
+        <v>8.1476394518133169E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2726,15 +3252,31 @@
         <v>0.32804057474462972</v>
       </c>
       <c r="E90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.14618622328384659</v>
       </c>
       <c r="F90">
         <f t="shared" si="3"/>
         <v>4.7955012705779808E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G90">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="5"/>
+        <v>0.34301598374820974</v>
+      </c>
+      <c r="I90">
+        <f>(1/(1+Imbal_Hasil))^G90</f>
+        <v>0.19563014309118829</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="6"/>
+        <v>6.7104265983226982E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -2750,15 +3292,31 @@
         <v>0.28228875578499624</v>
       </c>
       <c r="E91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.13791153139985526</v>
       </c>
       <c r="F91">
         <f t="shared" si="3"/>
         <v>3.893087460726858E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="5"/>
+        <v>0.29517554449484695</v>
+      </c>
+      <c r="I91">
+        <f>(1/(1+Imbal_Hasil))^G91</f>
+        <v>0.18455673876527198</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="6"/>
+        <v>5.4476635855232387E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2774,15 +3332,31 @@
         <v>0.23918043988906945</v>
       </c>
       <c r="E92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.13010521830175023</v>
       </c>
       <c r="F92">
         <f t="shared" si="3"/>
         <v>3.1118623345276028E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G92">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="5"/>
+        <v>0.25009928709503887</v>
+      </c>
+      <c r="I92">
+        <f>(1/(1+Imbal_Hasil))^G92</f>
+        <v>0.1741101309106339</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="6"/>
+        <v>4.3544819616773429E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -2798,15 +3372,31 @@
         <v>0.19933537040794938</v>
       </c>
       <c r="E93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.12274077198278321</v>
       </c>
       <c r="F93">
         <f t="shared" si="3"/>
         <v>2.4466577247345748E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="5"/>
+        <v>0.20843524685787632</v>
+      </c>
+      <c r="I93">
+        <f>(1/(1+Imbal_Hasil))^G93</f>
+        <v>0.16425484048173006</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="6"/>
+        <v>3.4236498223410503E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -2822,15 +3412,31 @@
         <v>0.16347294391785519</v>
       </c>
       <c r="E94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.11579318111583323</v>
       </c>
       <c r="F94">
         <f t="shared" si="3"/>
         <v>1.8929052202618653E-2</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="5"/>
+        <v>0.17093566159567578</v>
+      </c>
+      <c r="I94">
+        <f>(1/(1+Imbal_Hasil))^G94</f>
+        <v>0.15495739668087741</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="6"/>
+        <v>2.6487745120789354E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -2846,15 +3452,31 @@
         <v>0.13177554009218306</v>
       </c>
       <c r="E95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.1092388501092766</v>
       </c>
       <c r="F95">
         <f t="shared" si="3"/>
         <v>1.4395008472198954E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="5"/>
+        <v>0.13779123681227426</v>
+      </c>
+      <c r="I95">
+        <f>(1/(1+Imbal_Hasil))^G95</f>
+        <v>0.14618622328384659</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="6"/>
+        <v>2.0143180511196505E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -2870,15 +3492,31 @@
         <v>0.10426871385334079</v>
       </c>
       <c r="E96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.10305551897101564</v>
       </c>
       <c r="F96">
         <f t="shared" si="3"/>
         <v>1.0745466418596363E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G96">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="5"/>
+        <v>0.10902869404008013</v>
+      </c>
+      <c r="I96">
+        <f>(1/(1+Imbal_Hasil))^G96</f>
+        <v>0.13791153139985526</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="6"/>
+        <v>1.5036314161593723E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -2894,15 +3532,31 @@
         <v>8.0859344906127242E-2</v>
       </c>
       <c r="E97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.7222187708505312E-2</v>
       </c>
       <c r="F97">
         <f t="shared" si="3"/>
         <v>7.8613224084502758E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="5"/>
+        <v>8.4550661941141733E-2</v>
+      </c>
+      <c r="I97">
+        <f>(1/(1+Imbal_Hasil))^G97</f>
+        <v>0.13010521830175023</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="6"/>
+        <v>1.1000482329409729E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -2918,15 +3572,31 @@
         <v>6.1351219354074983E-2</v>
       </c>
       <c r="E98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.1719045008023872E-2</v>
       </c>
       <c r="F98">
         <f t="shared" si="3"/>
         <v>5.6270752492335483E-3</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G98">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="5"/>
+        <v>6.4151969241221879E-2</v>
+      </c>
+      <c r="I98">
+        <f>(1/(1+Imbal_Hasil))^G98</f>
+        <v>0.12274077198278321</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="6"/>
+        <v>7.874062228883337E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -2942,15 +3612,31 @@
         <v>4.55747532971746E-2</v>
       </c>
       <c r="E99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.6527400950965908E-2</v>
       </c>
       <c r="F99">
         <f t="shared" si="3"/>
         <v>3.9434649517859823E-3</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G99">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="5"/>
+        <v>4.7655290350841671E-2</v>
+      </c>
+      <c r="I99">
+        <f>(1/(1+Imbal_Hasil))^G99</f>
+        <v>0.11579318111583323</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="6"/>
+        <v>5.5181576667226295E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -2966,15 +3652,31 @@
         <v>3.3078611690622296E-2</v>
       </c>
       <c r="E100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.162962353864707E-2</v>
       </c>
       <c r="F100">
         <f t="shared" si="3"/>
         <v>2.7001946194865878E-3</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G100">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="5"/>
+        <v>3.4588686289544396E-2</v>
+      </c>
+      <c r="I100">
+        <f>(1/(1+Imbal_Hasil))^G100</f>
+        <v>0.1092388501092766</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="6"/>
+        <v>3.778428317060331E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
@@ -2990,15 +3692,31 @@
         <v>2.3403448557232181E-2</v>
       </c>
       <c r="E101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.7009078810044401E-2</v>
       </c>
       <c r="F101">
         <f t="shared" si="3"/>
         <v>1.802278014370713E-3</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G101">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="5"/>
+        <v>2.4471841436715554E-2</v>
+      </c>
+      <c r="I101">
+        <f>(1/(1+Imbal_Hasil))^G101</f>
+        <v>0.10305551897101564</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="6"/>
+        <v>2.5219583194371264E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -3014,15 +3732,31 @@
         <v>1.6098062090092156E-2</v>
       </c>
       <c r="E102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.2650074349098481E-2</v>
       </c>
       <c r="F102">
         <f t="shared" si="3"/>
         <v>1.1695254077215987E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G102">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="5"/>
+        <v>1.6832956132244795E-2</v>
+      </c>
+      <c r="I102">
+        <f>(1/(1+Imbal_Hasil))^G102</f>
+        <v>9.7222187708505312E-2</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="6"/>
+        <v>1.6365368207781389E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
@@ -3038,15 +3772,31 @@
         <v>1.0732417014843541E-2</v>
       </c>
       <c r="E103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6.8537805989715539E-2</v>
       </c>
       <c r="F103">
         <f t="shared" si="3"/>
         <v>7.3557631516406861E-4</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G103">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="5"/>
+        <v>1.1222363523806282E-2</v>
+      </c>
+      <c r="I103">
+        <f>(1/(1+Imbal_Hasil))^G103</f>
+        <v>9.1719045008023872E-2</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="6"/>
+        <v>1.0293044651363938E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
@@ -3062,15 +3812,31 @@
         <v>6.9585772199141057E-3</v>
       </c>
       <c r="E104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6.4658307537467472E-2</v>
       </c>
       <c r="F104">
         <f t="shared" si="3"/>
         <v>4.4992982590842169E-4</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G104">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="5"/>
+        <v>7.2762438379302789E-3</v>
+      </c>
+      <c r="I104">
+        <f>(1/(1+Imbal_Hasil))^G104</f>
+        <v>8.6527400950965908E-2</v>
+      </c>
+      <c r="J104">
+        <f t="shared" si="6"/>
+        <v>6.2959446798158819E-4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
@@ -3086,15 +3852,31 @@
         <v>4.3747183266155997E-3</v>
       </c>
       <c r="E105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6.0998403337233463E-2</v>
       </c>
       <c r="F105">
         <f t="shared" si="3"/>
         <v>2.6685083297368537E-4</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G105">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="5"/>
+        <v>4.5744289760300079E-3</v>
+      </c>
+      <c r="I105">
+        <f>(1/(1+Imbal_Hasil))^G105</f>
+        <v>8.162962353864707E-2</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="6"/>
+        <v>3.7340891521760834E-4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
@@ -3110,15 +3892,31 @@
         <v>2.6576413834189768E-3</v>
       </c>
       <c r="E106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5.7545663525691938E-2</v>
       </c>
       <c r="F106">
         <f t="shared" si="3"/>
         <v>1.5293573682218287E-4</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G106">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="5"/>
+        <v>2.7789656029382293E-3</v>
+      </c>
+      <c r="I106">
+        <f>(1/(1+Imbal_Hasil))^G106</f>
+        <v>7.7009078810044401E-2</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="6"/>
+        <v>2.1400558112707265E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
@@ -3134,15 +3932,31 @@
         <v>1.5540026461265781E-3</v>
       </c>
       <c r="E107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5.42883618166905E-2</v>
       </c>
       <c r="F107">
         <f t="shared" si="3"/>
         <v>8.4364257917014115E-5</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G107">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="5"/>
+        <v>1.6249445570060707E-3</v>
+      </c>
+      <c r="I107">
+        <f>(1/(1+Imbal_Hasil))^G107</f>
+        <v>7.2650074349098481E-2</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="6"/>
+        <v>1.1805234287965394E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
@@ -3158,15 +3972,31 @@
         <v>8.7066106254533805E-4</v>
       </c>
       <c r="E108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5.1215435676123106E-2</v>
       </c>
       <c r="F108">
         <f t="shared" si="3"/>
         <v>4.4591285644495755E-5</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G108">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="H108">
+        <f t="shared" si="5"/>
+        <v>9.1040768695379139E-4</v>
+      </c>
+      <c r="I108">
+        <f>(1/(1+Imbal_Hasil))^G108</f>
+        <v>6.8537805989715539E-2</v>
+      </c>
+      <c r="J108">
+        <f t="shared" si="6"/>
+        <v>6.2397345419984627E-5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
@@ -3182,15 +4012,31 @@
         <v>4.6491559417795965E-4</v>
       </c>
       <c r="E109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4.8316448751059525E-2</v>
       </c>
       <c r="F109">
         <f t="shared" si="3"/>
         <v>2.2463070479667775E-5</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G109">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="5"/>
+        <v>4.861394966795856E-4</v>
+      </c>
+      <c r="I109">
+        <f>(1/(1+Imbal_Hasil))^G109</f>
+        <v>6.4658307537467472E-2</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="6"/>
+        <v>3.1432957082418296E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
@@ -3206,15 +4052,31 @@
         <v>2.3511246513173599E-4</v>
       </c>
       <c r="E110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4.5581555425527859E-2</v>
       </c>
       <c r="F110">
         <f t="shared" si="3"/>
         <v>1.071679186063471E-5</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G110">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="5"/>
+        <v>2.4584560486583322E-4</v>
+      </c>
+      <c r="I110">
+        <f>(1/(1+Imbal_Hasil))^G110</f>
+        <v>6.0998403337233463E-2</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="6"/>
+        <v>1.499618936429222E-5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
@@ -3230,15 +4092,31 @@
         <v>1.1175600805106808E-4</v>
       </c>
       <c r="E111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4.300146738257344E-2</v>
       </c>
       <c r="F111">
         <f t="shared" si="3"/>
         <v>4.8056723350146186E-6</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G111">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="5"/>
+        <v>1.1685779136087652E-4</v>
+      </c>
+      <c r="I111">
+        <f>(1/(1+Imbal_Hasil))^G111</f>
+        <v>5.7545663525691938E-2</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="6"/>
+        <v>6.7246591420085105E-6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
@@ -3254,15 +4132,31 @@
         <v>4.947103208396631E-5</v>
       </c>
       <c r="E112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4.0567422059031535E-2</v>
       </c>
       <c r="F112">
         <f t="shared" si="3"/>
         <v>2.0069122382461519E-6</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G112">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="5"/>
+        <v>5.1729438501719214E-5</v>
+      </c>
+      <c r="I112">
+        <f>(1/(1+Imbal_Hasil))^G112</f>
+        <v>5.42883618166905E-2</v>
+      </c>
+      <c r="J112">
+        <f t="shared" si="6"/>
+        <v>2.808306473955573E-6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
@@ -3278,12 +4172,28 @@
         <v>2.0162413836141311E-5</v>
       </c>
       <c r="E113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.8271152885878811E-2</v>
       </c>
       <c r="F113">
         <f t="shared" si="3"/>
         <v>7.7163882247132233E-7</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="5"/>
+        <v>2.1082849955760683E-5</v>
+      </c>
+      <c r="I113">
+        <f>(1/(1+Imbal_Hasil))^G113</f>
+        <v>5.1215435676123106E-2</v>
+      </c>
+      <c r="J113">
+        <f t="shared" si="6"/>
+        <v>1.079767345778616E-6</v>
       </c>
     </row>
   </sheetData>
@@ -3293,10 +4203,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212A8B80-2381-44BF-B081-BA50A49CED38}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3337,8 +4247,8 @@
         <v>26</v>
       </c>
       <c r="B4" s="7">
-        <f>B2+B3</f>
-        <v>323489972.40786862</v>
+        <f>B2+B3+B18</f>
+        <v>863502846.70757413</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3356,7 +4266,7 @@
       </c>
       <c r="B7" s="7">
         <f>B4/(B6*12)</f>
-        <v>2015478.2641042208</v>
+        <v>5379985.0597436987</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3374,7 +4284,7 @@
       </c>
       <c r="B9" s="7">
         <f>B8-B7</f>
-        <v>11289662.084128534</v>
+        <v>7925155.2884890568</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3383,16 +4293,61 @@
       </c>
       <c r="B11" s="7">
         <f>B9*B6*12</f>
-        <v>1812022754.6646717</v>
+        <v>1272009880.3649659</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="11">
         <f>-PMT( (1+Imbal_Hasil)^(1/12)-1, Masa_Kerja*12, 0, B11 )</f>
-        <v>6315606.7734678816</v>
+        <v>4433451.0676924204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <f>Usia_Pensiun_JP</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <f>(Usia_Pensiun_JP - Usia_Mulai_Iuran_JP) * 12</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="10">
+        <f>MIN( (1% * Masa_Iuran_JP * (B1 * 12) / 12), Batas_Atas_Manfaat_JP )</f>
+        <v>4792300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="10">
+        <f>Manfaat_JP_Final * 12 * Faktor_Anuitas_60</f>
+        <v>722659040.62115991</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="10">
+        <f>B17 / (1 + Imbal_Hasil)^(Usia_Pensiun_JP - Usia_Pensiun)</f>
+        <v>540012874.29970551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated: memperdetail perhitungan Pesangon akibat pensiun
</commit_message>
<xml_diff>
--- a/case_study_IRR_rate/Draft Perhitungan.xlsx
+++ b/case_study_IRR_rate/Draft Perhitungan.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZakiZ\Downloads\teori dana pensiun\teori-dana-pensiun\case_study_IRR_rate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E59EA9-6278-4CA6-B57D-9D4FF8BFE8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69742E57-8744-44B5-8858-EF99F3E90DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{7B0AFCA6-860D-478D-9BA3-BF4DD6D924DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{7B0AFCA6-860D-478D-9BA3-BF4DD6D924DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Asumsi" sheetId="3" r:id="rId1"/>
     <sheet name="Proyeksi Tahunan" sheetId="1" r:id="rId2"/>
     <sheet name="Tabel Mortalita" sheetId="2" r:id="rId3"/>
-    <sheet name="Hasil &amp; Solusi" sheetId="4" r:id="rId4"/>
+    <sheet name="Referensi" sheetId="5" r:id="rId4"/>
+    <sheet name="Hasil &amp; Solusi" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Batas_Atas_Manfaat_JP">Asumsi!$B$15</definedName>
@@ -25,8 +26,8 @@
     <definedName name="Gender">Asumsi!$B$5</definedName>
     <definedName name="Imbal_Hasil">Asumsi!$B$7</definedName>
     <definedName name="Kenaikan_Gaji">Asumsi!$B$6</definedName>
-    <definedName name="Manfaat_JP_Final">'Hasil &amp; Solusi'!$B$16</definedName>
-    <definedName name="Masa_Iuran_JP">'Hasil &amp; Solusi'!$B$15</definedName>
+    <definedName name="Manfaat_JP_Final">'Hasil &amp; Solusi'!$B$20</definedName>
+    <definedName name="Masa_Iuran_JP">'Hasil &amp; Solusi'!$B$19</definedName>
     <definedName name="Masa_Kerja">Asumsi!$B$11</definedName>
     <definedName name="Rate_Iuran_JHT">Asumsi!$B$9</definedName>
     <definedName name="Target_IRR">Asumsi!$B$8</definedName>
@@ -55,30 +56,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Variabel Input</t>
   </si>
@@ -155,9 +134,6 @@
     <t>Total Akumulasi Dana JHT</t>
   </si>
   <si>
-    <t>Uang Pesangon (UUCK)</t>
-  </si>
-  <si>
     <t>TOTAL DANA LUMP SUM</t>
   </si>
   <si>
@@ -207,18 +183,40 @@
   </si>
   <si>
     <t>PV Manfaat JP di Usia 55</t>
+  </si>
+  <si>
+    <t>Faktor UP (Bulan)</t>
+  </si>
+  <si>
+    <t>Faktor UPMK (Bulan)</t>
+  </si>
+  <si>
+    <t>Faktor UP Pensiun (1.75x)</t>
+  </si>
+  <si>
+    <t>Faktor UPMK</t>
+  </si>
+  <si>
+    <t>Faktor UPH (15%)</t>
+  </si>
+  <si>
+    <t>Total Faktor Pengali Pesangon</t>
+  </si>
+  <si>
+    <t>Uang Pesangon Final (UUCK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$Rp-421]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$Rp-421]#,##0"/>
-    <numFmt numFmtId="173" formatCode="_-[$Rp-3809]* #,##0.00_-;\-[$Rp-3809]* #,##0.00_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-[$Rp-3809]* #,##0.00_-;\-[$Rp-3809]* #,##0.00_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +226,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -258,10 +263,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -280,10 +286,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,7 +726,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>60</v>
@@ -723,7 +734,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>25</v>
@@ -731,7 +742,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="10">
         <v>4792300</v>
@@ -1532,7 +1543,7 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1">
         <f>SUM(F57:F113)</f>
@@ -1547,7 +1558,7 @@
         <v>100000</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <f>SUM(J62:J113)</f>
@@ -2148,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="I62">
-        <f>(1/(1+Imbal_Hasil))^G62</f>
+        <f t="shared" ref="I62:I93" si="4">(1/(1+Imbal_Hasil))^G62</f>
         <v>1</v>
       </c>
       <c r="J62">
@@ -2188,7 +2199,7 @@
         <v>0.99000999999999995</v>
       </c>
       <c r="I63">
-        <f>(1/(1+Imbal_Hasil))^G63</f>
+        <f t="shared" si="4"/>
         <v>0.94339622641509424</v>
       </c>
       <c r="J63">
@@ -2220,19 +2231,19 @@
         <v>0.62322035496171879</v>
       </c>
       <c r="G64">
-        <f t="shared" ref="G64:G113" si="4">G63+1</f>
+        <f t="shared" ref="G64:G113" si="5">G63+1</f>
         <v>2</v>
       </c>
       <c r="H64">
-        <f t="shared" ref="H64:H113" si="5">B64/$B$62</f>
+        <f t="shared" ref="H64:H113" si="6">B64/$B$62</f>
         <v>0.97987229759999983</v>
       </c>
       <c r="I64">
-        <f>(1/(1+Imbal_Hasil))^G64</f>
+        <f t="shared" si="4"/>
         <v>0.88999644001423972</v>
       </c>
       <c r="J64">
-        <f t="shared" ref="J64:J113" si="6">I64*H64</f>
+        <f t="shared" ref="J64:J113" si="7">I64*H64</f>
         <v>0.87208285653257345</v>
       </c>
     </row>
@@ -2260,19 +2271,19 @@
         <v>0.58179383966869724</v>
       </c>
       <c r="G65">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="6"/>
+        <v>0.96962283336710375</v>
+      </c>
+      <c r="I65">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="H65">
-        <f t="shared" si="5"/>
-        <v>0.96962283336710375</v>
-      </c>
-      <c r="I65">
-        <f>(1/(1+Imbal_Hasil))^G65</f>
         <v>0.83961928303230149</v>
       </c>
       <c r="J65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.81411402816343637</v>
       </c>
     </row>
@@ -2300,19 +2311,19 @@
         <v>0.54298379966589194</v>
       </c>
       <c r="G66">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="6"/>
+        <v>0.95923817282174217</v>
+      </c>
+      <c r="I66">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="H66">
-        <f t="shared" si="5"/>
-        <v>0.95923817282174217</v>
-      </c>
-      <c r="I66">
-        <f>(1/(1+Imbal_Hasil))^G66</f>
         <v>0.79209366323802022</v>
       </c>
       <c r="J66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.75980647822811886</v>
       </c>
     </row>
@@ -2340,19 +2351,19 @@
         <v>0.506593640110925</v>
       </c>
       <c r="G67">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="6"/>
+        <v>0.94864818339379009</v>
+      </c>
+      <c r="I67">
         <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="H67">
-        <f t="shared" si="5"/>
-        <v>0.94864818339379009</v>
-      </c>
-      <c r="I67">
-        <f>(1/(1+Imbal_Hasil))^G67</f>
         <v>0.74725817286605678</v>
       </c>
       <c r="J67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.70888510821554751</v>
       </c>
     </row>
@@ -2380,19 +2391,19 @@
         <v>0.47244158207099402</v>
       </c>
       <c r="G68">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="6"/>
+        <v>0.93777667521209718</v>
+      </c>
+      <c r="I68">
         <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="H68">
-        <f t="shared" si="5"/>
-        <v>0.93777667521209718</v>
-      </c>
-      <c r="I68">
-        <f>(1/(1+Imbal_Hasil))^G68</f>
         <v>0.70496054043967604</v>
       </c>
       <c r="J68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.66109555176924262</v>
       </c>
     </row>
@@ -2420,19 +2431,19 @@
         <v>0.4403556674546818</v>
       </c>
       <c r="G69">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="6"/>
+        <v>0.92653273287630422</v>
+      </c>
+      <c r="I69">
         <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="5"/>
-        <v>0.92653273287630422</v>
-      </c>
-      <c r="I69">
-        <f>(1/(1+Imbal_Hasil))^G69</f>
         <v>0.66505711362233577</v>
       </c>
       <c r="J69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.61619718500332954</v>
       </c>
     </row>
@@ -2460,19 +2471,19 @@
         <v>0.41019545853278566</v>
       </c>
       <c r="G70">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="6"/>
+        <v>0.91485842044206278</v>
+      </c>
+      <c r="I70">
         <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="5"/>
-        <v>0.91485842044206278</v>
-      </c>
-      <c r="I70">
-        <f>(1/(1+Imbal_Hasil))^G70</f>
         <v>0.62741237134182615</v>
       </c>
       <c r="J70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.57399349101159203</v>
       </c>
     </row>
@@ -2500,19 +2511,19 @@
         <v>0.3818339253668725</v>
       </c>
       <c r="G71">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="6"/>
+        <v>0.90269995203438769</v>
+      </c>
+      <c r="I71">
         <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="H71">
-        <f t="shared" si="5"/>
-        <v>0.90269995203438769</v>
-      </c>
-      <c r="I71">
-        <f>(1/(1+Imbal_Hasil))^G71</f>
         <v>0.59189846353002462</v>
       </c>
       <c r="J71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.53430671463778101</v>
       </c>
     </row>
@@ -2540,19 +2551,19 @@
         <v>0.35515958369383754</v>
       </c>
       <c r="G72">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="6"/>
+        <v>0.89001701770830455</v>
+      </c>
+      <c r="I72">
         <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="H72">
-        <f t="shared" si="5"/>
-        <v>0.89001701770830455</v>
-      </c>
-      <c r="I72">
-        <f>(1/(1+Imbal_Hasil))^G72</f>
         <v>0.55839477691511752</v>
       </c>
       <c r="J72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.49698085405388692</v>
       </c>
     </row>
@@ -2580,19 +2591,19 @@
         <v>0.33008062629809815</v>
       </c>
       <c r="G73">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="6"/>
+        <v>0.87680026499533614</v>
+      </c>
+      <c r="I73">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="H73">
-        <f t="shared" si="5"/>
-        <v>0.87680026499533614</v>
-      </c>
-      <c r="I73">
-        <f>(1/(1+Imbal_Hasil))^G73</f>
         <v>0.52678752539162021</v>
       </c>
       <c r="J73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.46188744185960995</v>
       </c>
     </row>
@@ -2620,19 +2631,19 @@
         <v>0.30649543135864721</v>
       </c>
       <c r="G74">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="6"/>
+        <v>0.86299942882430958</v>
+      </c>
+      <c r="I74">
         <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="H74">
-        <f t="shared" si="5"/>
-        <v>0.86299942882430958</v>
-      </c>
-      <c r="I74">
-        <f>(1/(1+Imbal_Hasil))^G74</f>
         <v>0.49696936357700011</v>
       </c>
       <c r="J74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.42888427691013176</v>
       </c>
     </row>
@@ -2660,19 +2671,19 @@
         <v>0.28431788458014878</v>
       </c>
       <c r="G75">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="6"/>
+        <v>0.84858733836294353</v>
+      </c>
+      <c r="I75">
         <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="5"/>
-        <v>0.84858733836294353</v>
-      </c>
-      <c r="I75">
-        <f>(1/(1+Imbal_Hasil))^G75</f>
         <v>0.46883902224245294</v>
       </c>
       <c r="J75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.39785085800540804</v>
       </c>
     </row>
@@ -2700,19 +2711,19 @@
         <v>0.263458071482226</v>
       </c>
       <c r="G76">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="6"/>
+        <v>0.83350794136023409</v>
+      </c>
+      <c r="I76">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="5"/>
-        <v>0.83350794136023409</v>
-      </c>
-      <c r="I76">
-        <f>(1/(1+Imbal_Hasil))^G76</f>
         <v>0.44230096437967248</v>
       </c>
       <c r="J76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.36866136628174706</v>
       </c>
     </row>
@@ -2740,19 +2751,19 @@
         <v>0.24383541606380921</v>
       </c>
       <c r="G77">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="6"/>
+        <v>0.81771296587145759</v>
+      </c>
+      <c r="I77">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="5"/>
-        <v>0.81771296587145759</v>
-      </c>
-      <c r="I77">
-        <f>(1/(1+Imbal_Hasil))^G77</f>
         <v>0.41726506073553998</v>
       </c>
       <c r="J77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.34120305036859228</v>
       </c>
     </row>
@@ -2780,19 +2791,19 @@
         <v>0.22537293446637399</v>
       </c>
       <c r="G78">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="6"/>
+        <v>0.80114610118290186</v>
+      </c>
+      <c r="I78">
         <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="5"/>
-        <v>0.80114610118290186</v>
-      </c>
-      <c r="I78">
-        <f>(1/(1+Imbal_Hasil))^G78</f>
         <v>0.39364628371277355</v>
       </c>
       <c r="J78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.31536818544162698</v>
       </c>
     </row>
@@ -2820,19 +2831,19 @@
         <v>0.20757910344232597</v>
       </c>
       <c r="G79">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="6"/>
+        <v>0.78216695004587888</v>
+      </c>
+      <c r="I79">
         <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="5"/>
-        <v>0.78216695004587888</v>
-      </c>
-      <c r="I79">
-        <f>(1/(1+Imbal_Hasil))^G79</f>
         <v>0.37136441859695613</v>
       </c>
       <c r="J79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.29046897464954224</v>
       </c>
     </row>
@@ -2860,19 +2871,19 @@
         <v>0.19046753546233497</v>
       </c>
       <c r="G80">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="6"/>
+        <v>0.76075121895362274</v>
+      </c>
+      <c r="I80">
         <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="H80">
-        <f t="shared" si="5"/>
-        <v>0.76075121895362274</v>
-      </c>
-      <c r="I80">
-        <f>(1/(1+Imbal_Hasil))^G80</f>
         <v>0.35034379112920383</v>
       </c>
       <c r="J80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.26652446615437519</v>
       </c>
     </row>
@@ -2900,19 +2911,19 @@
         <v>0.17406217132298479</v>
       </c>
       <c r="G81">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="6"/>
+        <v>0.73693970580037438</v>
+      </c>
+      <c r="I81">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="H81">
-        <f t="shared" si="5"/>
-        <v>0.73693970580037438</v>
-      </c>
-      <c r="I81">
-        <f>(1/(1+Imbal_Hasil))^G81</f>
         <v>0.33051301049924886</v>
       </c>
       <c r="J81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.24356816072051252</v>
       </c>
     </row>
@@ -2940,19 +2951,19 @@
         <v>0.15814533522266697</v>
       </c>
       <c r="G82">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="6"/>
+        <v>0.7097245224651666</v>
+      </c>
+      <c r="I82">
         <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="H82">
-        <f t="shared" si="5"/>
-        <v>0.7097245224651666</v>
-      </c>
-      <c r="I82">
-        <f>(1/(1+Imbal_Hasil))^G82</f>
         <v>0.31180472688608379</v>
       </c>
       <c r="J82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.22129546089160751</v>
       </c>
     </row>
@@ -2980,19 +2991,19 @@
         <v>0.1424531405446291</v>
       </c>
       <c r="G83">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="6"/>
+        <v>0.67765916854019037</v>
+      </c>
+      <c r="I83">
         <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="H83">
-        <f t="shared" si="5"/>
-        <v>0.67765916854019037</v>
-      </c>
-      <c r="I83">
-        <f>(1/(1+Imbal_Hasil))^G83</f>
         <v>0.29415540272272056</v>
       </c>
       <c r="J83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.19933710563068366</v>
       </c>
     </row>
@@ -3020,19 +3031,19 @@
         <v>0.12696203345917681</v>
       </c>
       <c r="G84">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="6"/>
+        <v>0.64020494629497404</v>
+      </c>
+      <c r="I84">
         <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-      <c r="H84">
-        <f t="shared" si="5"/>
-        <v>0.64020494629497404</v>
-      </c>
-      <c r="I84">
-        <f>(1/(1+Imbal_Hasil))^G84</f>
         <v>0.27750509690822689</v>
       </c>
       <c r="J84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.17766013566271296</v>
       </c>
     </row>
@@ -3060,19 +3071,19 @@
         <v>0.11171221638368395</v>
       </c>
       <c r="G85">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="6"/>
+        <v>0.5971063493103963</v>
+      </c>
+      <c r="I85">
         <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
-      <c r="H85">
-        <f t="shared" si="5"/>
-        <v>0.5971063493103963</v>
-      </c>
-      <c r="I85">
-        <f>(1/(1+Imbal_Hasil))^G85</f>
         <v>0.26179726123417624</v>
       </c>
       <c r="J85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.15632080691499911</v>
       </c>
     </row>
@@ -3100,19 +3111,19 @@
         <v>9.6717486056258892E-2</v>
       </c>
       <c r="G86">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="6"/>
+        <v>0.54797643888913694</v>
+      </c>
+      <c r="I86">
         <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="H86">
-        <f t="shared" si="5"/>
-        <v>0.54797643888913694</v>
-      </c>
-      <c r="I86">
-        <f>(1/(1+Imbal_Hasil))^G86</f>
         <v>0.24697854833412852</v>
       </c>
       <c r="J86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.13533842539814434</v>
       </c>
     </row>
@@ -3140,19 +3151,19 @@
         <v>8.2594908233817613E-2</v>
       </c>
       <c r="G87">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="6"/>
+        <v>0.49603923201122452</v>
+      </c>
+      <c r="I87">
         <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-      <c r="H87">
-        <f t="shared" si="5"/>
-        <v>0.49603923201122452</v>
-      </c>
-      <c r="I87">
-        <f>(1/(1+Imbal_Hasil))^G87</f>
         <v>0.23299863050389483</v>
       </c>
       <c r="J87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.11557646173481906</v>
       </c>
     </row>
@@ -3180,19 +3191,19 @@
         <v>6.9765425553913768E-2</v>
       </c>
       <c r="G88">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="6"/>
+        <v>0.44412872638124989</v>
+      </c>
+      <c r="I88">
         <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="H88">
-        <f t="shared" si="5"/>
-        <v>0.44412872638124989</v>
-      </c>
-      <c r="I88">
-        <f>(1/(1+Imbal_Hasil))^G88</f>
         <v>0.21981002877725925</v>
       </c>
       <c r="J88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.7623948126670038E-2</v>
       </c>
     </row>
@@ -3212,7 +3223,7 @@
         <v>0.37575379114410867</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89:E113" si="7">(1/(1+Imbal_Hasil))^C89</f>
+        <f t="shared" ref="E89:E113" si="8">(1/(1+Imbal_Hasil))^C89</f>
         <v>0.15495739668087741</v>
       </c>
       <c r="F89">
@@ -3220,19 +3231,19 @@
         <v>5.8225829268661211E-2</v>
       </c>
       <c r="G89">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="6"/>
+        <v>0.3929073603677003</v>
+      </c>
+      <c r="I89">
         <f t="shared" si="4"/>
-        <v>27</v>
-      </c>
-      <c r="H89">
-        <f t="shared" si="5"/>
-        <v>0.3929073603677003</v>
-      </c>
-      <c r="I89">
-        <f>(1/(1+Imbal_Hasil))^G89</f>
         <v>0.20736795167665964</v>
       </c>
       <c r="J89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.1476394518133169E-2</v>
       </c>
     </row>
@@ -3252,7 +3263,7 @@
         <v>0.32804057474462972</v>
       </c>
       <c r="E90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.14618622328384659</v>
       </c>
       <c r="F90">
@@ -3260,19 +3271,19 @@
         <v>4.7955012705779808E-2</v>
       </c>
       <c r="G90">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="6"/>
+        <v>0.34301598374820974</v>
+      </c>
+      <c r="I90">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="H90">
-        <f t="shared" si="5"/>
-        <v>0.34301598374820974</v>
-      </c>
-      <c r="I90">
-        <f>(1/(1+Imbal_Hasil))^G90</f>
         <v>0.19563014309118829</v>
       </c>
       <c r="J90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.7104265983226982E-2</v>
       </c>
     </row>
@@ -3292,7 +3303,7 @@
         <v>0.28228875578499624</v>
       </c>
       <c r="E91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.13791153139985526</v>
       </c>
       <c r="F91">
@@ -3300,19 +3311,19 @@
         <v>3.893087460726858E-2</v>
       </c>
       <c r="G91">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="6"/>
+        <v>0.29517554449484695</v>
+      </c>
+      <c r="I91">
         <f t="shared" si="4"/>
-        <v>29</v>
-      </c>
-      <c r="H91">
-        <f t="shared" si="5"/>
-        <v>0.29517554449484695</v>
-      </c>
-      <c r="I91">
-        <f>(1/(1+Imbal_Hasil))^G91</f>
         <v>0.18455673876527198</v>
       </c>
       <c r="J91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.4476635855232387E-2</v>
       </c>
     </row>
@@ -3332,7 +3343,7 @@
         <v>0.23918043988906945</v>
       </c>
       <c r="E92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.13010521830175023</v>
       </c>
       <c r="F92">
@@ -3340,19 +3351,19 @@
         <v>3.1118623345276028E-2</v>
       </c>
       <c r="G92">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="6"/>
+        <v>0.25009928709503887</v>
+      </c>
+      <c r="I92">
         <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="H92">
-        <f t="shared" si="5"/>
-        <v>0.25009928709503887</v>
-      </c>
-      <c r="I92">
-        <f>(1/(1+Imbal_Hasil))^G92</f>
         <v>0.1741101309106339</v>
       </c>
       <c r="J92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.3544819616773429E-2</v>
       </c>
     </row>
@@ -3372,7 +3383,7 @@
         <v>0.19933537040794938</v>
       </c>
       <c r="E93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.12274077198278321</v>
       </c>
       <c r="F93">
@@ -3380,19 +3391,19 @@
         <v>2.4466577247345748E-2</v>
       </c>
       <c r="G93">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="6"/>
+        <v>0.20843524685787632</v>
+      </c>
+      <c r="I93">
         <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="H93">
-        <f t="shared" si="5"/>
-        <v>0.20843524685787632</v>
-      </c>
-      <c r="I93">
-        <f>(1/(1+Imbal_Hasil))^G93</f>
         <v>0.16425484048173006</v>
       </c>
       <c r="J93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.4236498223410503E-2</v>
       </c>
     </row>
@@ -3412,7 +3423,7 @@
         <v>0.16347294391785519</v>
       </c>
       <c r="E94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.11579318111583323</v>
       </c>
       <c r="F94">
@@ -3420,19 +3431,19 @@
         <v>1.8929052202618653E-2</v>
       </c>
       <c r="G94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="H94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.17093566159567578</v>
       </c>
       <c r="I94">
-        <f>(1/(1+Imbal_Hasil))^G94</f>
+        <f t="shared" ref="I94:I113" si="9">(1/(1+Imbal_Hasil))^G94</f>
         <v>0.15495739668087741</v>
       </c>
       <c r="J94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.6487745120789354E-2</v>
       </c>
     </row>
@@ -3452,7 +3463,7 @@
         <v>0.13177554009218306</v>
       </c>
       <c r="E95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1092388501092766</v>
       </c>
       <c r="F95">
@@ -3460,19 +3471,19 @@
         <v>1.4395008472198954E-2</v>
       </c>
       <c r="G95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="H95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.13779123681227426</v>
       </c>
       <c r="I95">
-        <f>(1/(1+Imbal_Hasil))^G95</f>
+        <f t="shared" si="9"/>
         <v>0.14618622328384659</v>
       </c>
       <c r="J95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.0143180511196505E-2</v>
       </c>
     </row>
@@ -3492,7 +3503,7 @@
         <v>0.10426871385334079</v>
       </c>
       <c r="E96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.10305551897101564</v>
       </c>
       <c r="F96">
@@ -3500,19 +3511,19 @@
         <v>1.0745466418596363E-2</v>
       </c>
       <c r="G96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="H96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.10902869404008013</v>
       </c>
       <c r="I96">
-        <f>(1/(1+Imbal_Hasil))^G96</f>
+        <f t="shared" si="9"/>
         <v>0.13791153139985526</v>
       </c>
       <c r="J96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5036314161593723E-2</v>
       </c>
     </row>
@@ -3532,7 +3543,7 @@
         <v>8.0859344906127242E-2</v>
       </c>
       <c r="E97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.7222187708505312E-2</v>
       </c>
       <c r="F97">
@@ -3540,19 +3551,19 @@
         <v>7.8613224084502758E-3</v>
       </c>
       <c r="G97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="H97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.4550661941141733E-2</v>
       </c>
       <c r="I97">
-        <f>(1/(1+Imbal_Hasil))^G97</f>
+        <f t="shared" si="9"/>
         <v>0.13010521830175023</v>
       </c>
       <c r="J97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1000482329409729E-2</v>
       </c>
     </row>
@@ -3572,7 +3583,7 @@
         <v>6.1351219354074983E-2</v>
       </c>
       <c r="E98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.1719045008023872E-2</v>
       </c>
       <c r="F98">
@@ -3580,19 +3591,19 @@
         <v>5.6270752492335483E-3</v>
       </c>
       <c r="G98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="H98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.4151969241221879E-2</v>
       </c>
       <c r="I98">
-        <f>(1/(1+Imbal_Hasil))^G98</f>
+        <f t="shared" si="9"/>
         <v>0.12274077198278321</v>
       </c>
       <c r="J98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.874062228883337E-3</v>
       </c>
     </row>
@@ -3612,7 +3623,7 @@
         <v>4.55747532971746E-2</v>
       </c>
       <c r="E99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8.6527400950965908E-2</v>
       </c>
       <c r="F99">
@@ -3620,19 +3631,19 @@
         <v>3.9434649517859823E-3</v>
       </c>
       <c r="G99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="H99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.7655290350841671E-2</v>
       </c>
       <c r="I99">
-        <f>(1/(1+Imbal_Hasil))^G99</f>
+        <f t="shared" si="9"/>
         <v>0.11579318111583323</v>
       </c>
       <c r="J99">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.5181576667226295E-3</v>
       </c>
     </row>
@@ -3652,7 +3663,7 @@
         <v>3.3078611690622296E-2</v>
       </c>
       <c r="E100">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8.162962353864707E-2</v>
       </c>
       <c r="F100">
@@ -3660,19 +3671,19 @@
         <v>2.7001946194865878E-3</v>
       </c>
       <c r="G100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="H100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.4588686289544396E-2</v>
       </c>
       <c r="I100">
-        <f>(1/(1+Imbal_Hasil))^G100</f>
+        <f t="shared" si="9"/>
         <v>0.1092388501092766</v>
       </c>
       <c r="J100">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.778428317060331E-3</v>
       </c>
     </row>
@@ -3692,7 +3703,7 @@
         <v>2.3403448557232181E-2</v>
       </c>
       <c r="E101">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.7009078810044401E-2</v>
       </c>
       <c r="F101">
@@ -3700,19 +3711,19 @@
         <v>1.802278014370713E-3</v>
       </c>
       <c r="G101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="H101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.4471841436715554E-2</v>
       </c>
       <c r="I101">
-        <f>(1/(1+Imbal_Hasil))^G101</f>
+        <f t="shared" si="9"/>
         <v>0.10305551897101564</v>
       </c>
       <c r="J101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5219583194371264E-3</v>
       </c>
     </row>
@@ -3732,7 +3743,7 @@
         <v>1.6098062090092156E-2</v>
       </c>
       <c r="E102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.2650074349098481E-2</v>
       </c>
       <c r="F102">
@@ -3740,19 +3751,19 @@
         <v>1.1695254077215987E-3</v>
       </c>
       <c r="G102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="H102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6832956132244795E-2</v>
       </c>
       <c r="I102">
-        <f>(1/(1+Imbal_Hasil))^G102</f>
+        <f t="shared" si="9"/>
         <v>9.7222187708505312E-2</v>
       </c>
       <c r="J102">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6365368207781389E-3</v>
       </c>
     </row>
@@ -3772,7 +3783,7 @@
         <v>1.0732417014843541E-2</v>
       </c>
       <c r="E103">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.8537805989715539E-2</v>
       </c>
       <c r="F103">
@@ -3780,19 +3791,19 @@
         <v>7.3557631516406861E-4</v>
       </c>
       <c r="G103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="H103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1222363523806282E-2</v>
       </c>
       <c r="I103">
-        <f>(1/(1+Imbal_Hasil))^G103</f>
+        <f t="shared" si="9"/>
         <v>9.1719045008023872E-2</v>
       </c>
       <c r="J103">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0293044651363938E-3</v>
       </c>
     </row>
@@ -3812,7 +3823,7 @@
         <v>6.9585772199141057E-3</v>
       </c>
       <c r="E104">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.4658307537467472E-2</v>
       </c>
       <c r="F104">
@@ -3820,19 +3831,19 @@
         <v>4.4992982590842169E-4</v>
       </c>
       <c r="G104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="H104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.2762438379302789E-3</v>
       </c>
       <c r="I104">
-        <f>(1/(1+Imbal_Hasil))^G104</f>
+        <f t="shared" si="9"/>
         <v>8.6527400950965908E-2</v>
       </c>
       <c r="J104">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.2959446798158819E-4</v>
       </c>
     </row>
@@ -3852,7 +3863,7 @@
         <v>4.3747183266155997E-3</v>
       </c>
       <c r="E105">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.0998403337233463E-2</v>
       </c>
       <c r="F105">
@@ -3860,19 +3871,19 @@
         <v>2.6685083297368537E-4</v>
       </c>
       <c r="G105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="H105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5744289760300079E-3</v>
       </c>
       <c r="I105">
-        <f>(1/(1+Imbal_Hasil))^G105</f>
+        <f t="shared" si="9"/>
         <v>8.162962353864707E-2</v>
       </c>
       <c r="J105">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.7340891521760834E-4</v>
       </c>
     </row>
@@ -3892,7 +3903,7 @@
         <v>2.6576413834189768E-3</v>
       </c>
       <c r="E106">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.7545663525691938E-2</v>
       </c>
       <c r="F106">
@@ -3900,19 +3911,19 @@
         <v>1.5293573682218287E-4</v>
       </c>
       <c r="G106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="H106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.7789656029382293E-3</v>
       </c>
       <c r="I106">
-        <f>(1/(1+Imbal_Hasil))^G106</f>
+        <f t="shared" si="9"/>
         <v>7.7009078810044401E-2</v>
       </c>
       <c r="J106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1400558112707265E-4</v>
       </c>
     </row>
@@ -3932,7 +3943,7 @@
         <v>1.5540026461265781E-3</v>
       </c>
       <c r="E107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.42883618166905E-2</v>
       </c>
       <c r="F107">
@@ -3940,19 +3951,19 @@
         <v>8.4364257917014115E-5</v>
       </c>
       <c r="G107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="H107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6249445570060707E-3</v>
       </c>
       <c r="I107">
-        <f>(1/(1+Imbal_Hasil))^G107</f>
+        <f t="shared" si="9"/>
         <v>7.2650074349098481E-2</v>
       </c>
       <c r="J107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1805234287965394E-4</v>
       </c>
     </row>
@@ -3972,7 +3983,7 @@
         <v>8.7066106254533805E-4</v>
       </c>
       <c r="E108">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.1215435676123106E-2</v>
       </c>
       <c r="F108">
@@ -3980,19 +3991,19 @@
         <v>4.4591285644495755E-5</v>
       </c>
       <c r="G108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="H108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.1040768695379139E-4</v>
       </c>
       <c r="I108">
-        <f>(1/(1+Imbal_Hasil))^G108</f>
+        <f t="shared" si="9"/>
         <v>6.8537805989715539E-2</v>
       </c>
       <c r="J108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.2397345419984627E-5</v>
       </c>
     </row>
@@ -4012,7 +4023,7 @@
         <v>4.6491559417795965E-4</v>
       </c>
       <c r="E109">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.8316448751059525E-2</v>
       </c>
       <c r="F109">
@@ -4020,19 +4031,19 @@
         <v>2.2463070479667775E-5</v>
       </c>
       <c r="G109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="H109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.861394966795856E-4</v>
       </c>
       <c r="I109">
-        <f>(1/(1+Imbal_Hasil))^G109</f>
+        <f t="shared" si="9"/>
         <v>6.4658307537467472E-2</v>
       </c>
       <c r="J109">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1432957082418296E-5</v>
       </c>
     </row>
@@ -4052,7 +4063,7 @@
         <v>2.3511246513173599E-4</v>
       </c>
       <c r="E110">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.5581555425527859E-2</v>
       </c>
       <c r="F110">
@@ -4060,19 +4071,19 @@
         <v>1.071679186063471E-5</v>
       </c>
       <c r="G110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="H110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.4584560486583322E-4</v>
       </c>
       <c r="I110">
-        <f>(1/(1+Imbal_Hasil))^G110</f>
+        <f t="shared" si="9"/>
         <v>6.0998403337233463E-2</v>
       </c>
       <c r="J110">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.499618936429222E-5</v>
       </c>
     </row>
@@ -4092,7 +4103,7 @@
         <v>1.1175600805106808E-4</v>
       </c>
       <c r="E111">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.300146738257344E-2</v>
       </c>
       <c r="F111">
@@ -4100,19 +4111,19 @@
         <v>4.8056723350146186E-6</v>
       </c>
       <c r="G111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
       <c r="H111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1685779136087652E-4</v>
       </c>
       <c r="I111">
-        <f>(1/(1+Imbal_Hasil))^G111</f>
+        <f t="shared" si="9"/>
         <v>5.7545663525691938E-2</v>
       </c>
       <c r="J111">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.7246591420085105E-6</v>
       </c>
     </row>
@@ -4132,7 +4143,7 @@
         <v>4.947103208396631E-5</v>
       </c>
       <c r="E112">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.0567422059031535E-2</v>
       </c>
       <c r="F112">
@@ -4140,19 +4151,19 @@
         <v>2.0069122382461519E-6</v>
       </c>
       <c r="G112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="H112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.1729438501719214E-5</v>
       </c>
       <c r="I112">
-        <f>(1/(1+Imbal_Hasil))^G112</f>
+        <f t="shared" si="9"/>
         <v>5.42883618166905E-2</v>
       </c>
       <c r="J112">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.808306473955573E-6</v>
       </c>
     </row>
@@ -4172,7 +4183,7 @@
         <v>2.0162413836141311E-5</v>
       </c>
       <c r="E113">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.8271152885878811E-2</v>
       </c>
       <c r="F113">
@@ -4180,19 +4191,19 @@
         <v>7.7163882247132233E-7</v>
       </c>
       <c r="G113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51</v>
       </c>
       <c r="H113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.1082849955760683E-5</v>
       </c>
       <c r="I113">
-        <f>(1/(1+Imbal_Hasil))^G113</f>
+        <f t="shared" si="9"/>
         <v>5.1215435676123106E-2</v>
       </c>
       <c r="J113">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.079767345778616E-6</v>
       </c>
     </row>
@@ -4202,11 +4213,170 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C507D4-5449-44FA-ADB1-87217C92C470}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212A8B80-2381-44BF-B081-BA50A49CED38}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4235,118 +4405,154 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="7" cm="1">
-        <f t="array" ref="B3">IF(Masa_Kerja&gt;=15, 9, 0) * B1</f>
-        <v>149682828.91761848</v>
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <f>VLOOKUP(Masa_Kerja, Referensi!$A$2:$B$10, 2, TRUE) * 1.75</f>
+        <v>15.75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="7">
-        <f>B2+B3+B18</f>
-        <v>863502846.70757413</v>
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <f>VLOOKUP(Masa_Kerja, Referensi!$D$2:$E$11, 2, TRUE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <f>0.15 * (B3 + B4)</f>
+        <v>3.2624999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <f>SUM(B3:B5)</f>
+        <v>25.012499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="13">
+        <f>B6 * B1</f>
+        <v>415993528.70021474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7">
+        <f>B2+B7+B22</f>
+        <v>1129813546.4901705</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="9">
         <f>'Tabel Mortalita'!E1</f>
         <v>13.375236131676656</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="7">
+        <f>B8/(B10*12)</f>
+        <v>7039212.463038478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="7">
-        <f>B4/(B6*12)</f>
-        <v>5379985.0597436987</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="B12" s="7">
         <f>B1*Target_IRR</f>
         <v>13305140.348232755</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7">
+        <f>B12-B11</f>
+        <v>6265927.8851942774</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="7">
-        <f>B8-B7</f>
-        <v>7925155.2884890568</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B15" s="7">
+        <f>B13*B10*12</f>
+        <v>1005699180.5823696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="7">
-        <f>B9*B6*12</f>
-        <v>1272009880.3649659</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="11">
-        <f>-PMT( (1+Imbal_Hasil)^(1/12)-1, Masa_Kerja*12, 0, B11 )</f>
-        <v>4433451.0676924204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14">
+      <c r="B16" s="11">
+        <f>-PMT( (1+Imbal_Hasil)^(1/12)-1, Masa_Kerja*12, 0, B15 )</f>
+        <v>3505254.3024673681</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18">
         <f>Usia_Pensiun_JP</f>
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
         <f>(Usia_Pensiun_JP - Usia_Mulai_Iuran_JP) * 12</f>
         <v>420</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="10">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="10">
         <f>MIN( (1% * Masa_Iuran_JP * (B1 * 12) / 12), Batas_Atas_Manfaat_JP )</f>
         <v>4792300</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="10">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="10">
         <f>Manfaat_JP_Final * 12 * Faktor_Anuitas_60</f>
         <v>722659040.62115991</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="10">
-        <f>B17 / (1 + Imbal_Hasil)^(Usia_Pensiun_JP - Usia_Pensiun)</f>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="10">
+        <f>B21 / (1 + Imbal_Hasil)^(Usia_Pensiun_JP - Usia_Pensiun)</f>
         <v>540012874.29970551</v>
       </c>
     </row>

</xml_diff>